<commit_message>
Minor cleanup to Tray 5 BOM.xlsx (erroneous description for R4)
git-svn-id: svn+ssh://localhost/home/pcb/svn@576 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/Bill of Materials masterlist/Internal/Tray 5/Interconnect/Tray 5 BOM.xlsx
+++ b/Bill of Materials masterlist/Internal/Tray 5/Interconnect/Tray 5 BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>1.5</t>
-  </si>
-  <si>
-    <t>0603 Thick Film Resistor 1%</t>
   </si>
   <si>
     <t>RMCF0805JT4K70CT-ND</t>
@@ -560,7 +557,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -808,7 +805,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -823,13 +820,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -849,13 +846,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -875,18 +872,18 @@
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -901,10 +898,10 @@
         <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>9</v>
@@ -912,7 +909,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -927,10 +924,10 @@
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>9</v>
@@ -938,7 +935,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -953,10 +950,10 @@
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>9</v>
@@ -964,7 +961,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -979,10 +976,10 @@
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>9</v>

</xml_diff>